<commit_message>
Successful PATCH request (had to change json parameter to data within request)
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PriceList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94644C33-8AED-449B-86F1-980C7F40F9EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC80696-7056-4250-B446-2B8A160F3424}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>aa</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>ItemCode</t>
   </si>
@@ -46,6 +40,333 @@
   </si>
   <si>
     <t>Price4</t>
+  </si>
+  <si>
+    <t>A00001</t>
+  </si>
+  <si>
+    <t>A00002</t>
+  </si>
+  <si>
+    <t>A00003</t>
+  </si>
+  <si>
+    <t>A00004</t>
+  </si>
+  <si>
+    <t>A00005</t>
+  </si>
+  <si>
+    <t>A00006</t>
+  </si>
+  <si>
+    <t>A00007</t>
+  </si>
+  <si>
+    <t>A00008</t>
+  </si>
+  <si>
+    <t>A00009</t>
+  </si>
+  <si>
+    <t>A00010</t>
+  </si>
+  <si>
+    <t>A00011</t>
+  </si>
+  <si>
+    <t>A00012</t>
+  </si>
+  <si>
+    <t>B10000</t>
+  </si>
+  <si>
+    <t>c000001</t>
+  </si>
+  <si>
+    <t>C00001</t>
+  </si>
+  <si>
+    <t>C00002</t>
+  </si>
+  <si>
+    <t>C00003</t>
+  </si>
+  <si>
+    <t>C00004</t>
+  </si>
+  <si>
+    <t>C00005</t>
+  </si>
+  <si>
+    <t>C00006</t>
+  </si>
+  <si>
+    <t>C00007</t>
+  </si>
+  <si>
+    <t>C00008</t>
+  </si>
+  <si>
+    <t>C00009</t>
+  </si>
+  <si>
+    <t>C00010</t>
+  </si>
+  <si>
+    <t>C00011</t>
+  </si>
+  <si>
+    <t>C00012</t>
+  </si>
+  <si>
+    <t>C00013</t>
+  </si>
+  <si>
+    <t>C00014</t>
+  </si>
+  <si>
+    <t>C00015</t>
+  </si>
+  <si>
+    <t>CPA7</t>
+  </si>
+  <si>
+    <t>CUT0001</t>
+  </si>
+  <si>
+    <t>D00001</t>
+  </si>
+  <si>
+    <t>D00002</t>
+  </si>
+  <si>
+    <t>E00001</t>
+  </si>
+  <si>
+    <t>FA00001</t>
+  </si>
+  <si>
+    <t>FA00002</t>
+  </si>
+  <si>
+    <t>I00001</t>
+  </si>
+  <si>
+    <t>I00002</t>
+  </si>
+  <si>
+    <t>I00003</t>
+  </si>
+  <si>
+    <t>I00004</t>
+  </si>
+  <si>
+    <t>I00005</t>
+  </si>
+  <si>
+    <t>I00006</t>
+  </si>
+  <si>
+    <t>I00007</t>
+  </si>
+  <si>
+    <t>I00008</t>
+  </si>
+  <si>
+    <t>I00009</t>
+  </si>
+  <si>
+    <t>I00010</t>
+  </si>
+  <si>
+    <t>I00011</t>
+  </si>
+  <si>
+    <t>I00012</t>
+  </si>
+  <si>
+    <t>I00013</t>
+  </si>
+  <si>
+    <t>L10001</t>
+  </si>
+  <si>
+    <t>label3565</t>
+  </si>
+  <si>
+    <t>LB0001</t>
+  </si>
+  <si>
+    <t>LB0002</t>
+  </si>
+  <si>
+    <t>LM4029</t>
+  </si>
+  <si>
+    <t>LM4029ACA</t>
+  </si>
+  <si>
+    <t>LM4029APCD</t>
+  </si>
+  <si>
+    <t>LM4029D</t>
+  </si>
+  <si>
+    <t>LM4029MC</t>
+  </si>
+  <si>
+    <t>LM4029PH</t>
+  </si>
+  <si>
+    <t>LM4029PS</t>
+  </si>
+  <si>
+    <t>LM4029SB</t>
+  </si>
+  <si>
+    <t>M00001</t>
+  </si>
+  <si>
+    <t>P10001</t>
+  </si>
+  <si>
+    <t>P10002</t>
+  </si>
+  <si>
+    <t>P10003</t>
+  </si>
+  <si>
+    <t>P10004</t>
+  </si>
+  <si>
+    <t>P20001</t>
+  </si>
+  <si>
+    <t>P20002</t>
+  </si>
+  <si>
+    <t>P20003</t>
+  </si>
+  <si>
+    <t>PC00001</t>
+  </si>
+  <si>
+    <t>PC00002</t>
+  </si>
+  <si>
+    <t>PC00003</t>
+  </si>
+  <si>
+    <t>PC00004</t>
+  </si>
+  <si>
+    <t>PC00005</t>
+  </si>
+  <si>
+    <t>PC00006</t>
+  </si>
+  <si>
+    <t>PC00007</t>
+  </si>
+  <si>
+    <t>PP01</t>
+  </si>
+  <si>
+    <t>PPR01</t>
+  </si>
+  <si>
+    <t>Printing0001</t>
+  </si>
+  <si>
+    <t>R00001</t>
+  </si>
+  <si>
+    <t>R00002</t>
+  </si>
+  <si>
+    <t>REF0001</t>
+  </si>
+  <si>
+    <t>REF0002</t>
+  </si>
+  <si>
+    <t>REF0003</t>
+  </si>
+  <si>
+    <t>REF0004</t>
+  </si>
+  <si>
+    <t>REF0005</t>
+  </si>
+  <si>
+    <t>S10000</t>
+  </si>
+  <si>
+    <t>St01</t>
+  </si>
+  <si>
+    <t>TAPE05217</t>
+  </si>
+  <si>
+    <t>TESA 52015</t>
+  </si>
+  <si>
+    <t>Tovar</t>
+  </si>
+  <si>
+    <t>TR0001</t>
+  </si>
+  <si>
+    <t>U00001</t>
+  </si>
+  <si>
+    <t>U0002</t>
+  </si>
+  <si>
+    <t>Z00001</t>
+  </si>
+  <si>
+    <t>Z00002</t>
+  </si>
+  <si>
+    <t>Бр01</t>
+  </si>
+  <si>
+    <t>БУМСАМ00001</t>
+  </si>
+  <si>
+    <t>ГП</t>
+  </si>
+  <si>
+    <t>ГП00001</t>
+  </si>
+  <si>
+    <t>ГП00002</t>
+  </si>
+  <si>
+    <t>ГСМ00001</t>
+  </si>
+  <si>
+    <t>КП0001</t>
+  </si>
+  <si>
+    <t>Н0001</t>
+  </si>
+  <si>
+    <t>ОС0001</t>
+  </si>
+  <si>
+    <t>ОС00050</t>
+  </si>
+  <si>
+    <t>С00008</t>
+  </si>
+  <si>
+    <t>СUT00001</t>
+  </si>
+  <si>
+    <t>УФ00001</t>
   </si>
 </sst>
 </file>
@@ -363,34 +684,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -407,7 +728,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -424,24 +745,18 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>13</v>
       </c>
       <c r="D4">
         <v>12</v>
-      </c>
-      <c r="E4">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -458,16 +773,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>12</v>
       </c>
       <c r="C6">
         <v>13</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
       </c>
       <c r="E6">
         <v>13</v>
@@ -475,7 +787,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -492,7 +804,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -509,13 +821,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>12</v>
-      </c>
-      <c r="C9">
-        <v>13</v>
       </c>
       <c r="D9">
         <v>12</v>
@@ -526,7 +835,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -543,10 +852,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>13</v>
@@ -560,7 +866,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>12</v>
@@ -572,6 +878,1537 @@
         <v>12</v>
       </c>
       <c r="E12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="E17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+      <c r="E21">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>12</v>
+      </c>
+      <c r="E22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>12</v>
+      </c>
+      <c r="C25">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>12</v>
+      </c>
+      <c r="C27">
+        <v>13</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
+        <v>12</v>
+      </c>
+      <c r="C28">
+        <v>13</v>
+      </c>
+      <c r="E28">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>13</v>
+      </c>
+      <c r="D29">
+        <v>12</v>
+      </c>
+      <c r="E29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
+        <v>12</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="D31">
+        <v>12</v>
+      </c>
+      <c r="E31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>13</v>
+      </c>
+      <c r="D33">
+        <v>12</v>
+      </c>
+      <c r="E33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>12</v>
+      </c>
+      <c r="E34">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>13</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>13</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="E39">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>13</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>13</v>
+      </c>
+      <c r="D41">
+        <v>12</v>
+      </c>
+      <c r="E41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>13</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+      <c r="E43">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>13</v>
+      </c>
+      <c r="D45">
+        <v>12</v>
+      </c>
+      <c r="E45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B46">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>13</v>
+      </c>
+      <c r="D46">
+        <v>12</v>
+      </c>
+      <c r="E46">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>12</v>
+      </c>
+      <c r="C47">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>12</v>
+      </c>
+      <c r="E47">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48">
+        <v>13</v>
+      </c>
+      <c r="D48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <v>12</v>
+      </c>
+      <c r="C49">
+        <v>13</v>
+      </c>
+      <c r="D49">
+        <v>12</v>
+      </c>
+      <c r="E49">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50">
+        <v>12</v>
+      </c>
+      <c r="C50">
+        <v>13</v>
+      </c>
+      <c r="E50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>12</v>
+      </c>
+      <c r="C51">
+        <v>13</v>
+      </c>
+      <c r="D51">
+        <v>12</v>
+      </c>
+      <c r="E51">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52">
+        <v>12</v>
+      </c>
+      <c r="C52">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>12</v>
+      </c>
+      <c r="E52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>12</v>
+      </c>
+      <c r="D53">
+        <v>12</v>
+      </c>
+      <c r="E53">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54">
+        <v>12</v>
+      </c>
+      <c r="C54">
+        <v>13</v>
+      </c>
+      <c r="D54">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55">
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>12</v>
+      </c>
+      <c r="E55">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>59</v>
+      </c>
+      <c r="B56">
+        <v>12</v>
+      </c>
+      <c r="C56">
+        <v>13</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>60</v>
+      </c>
+      <c r="B57">
+        <v>12</v>
+      </c>
+      <c r="C57">
+        <v>13</v>
+      </c>
+      <c r="D57">
+        <v>12</v>
+      </c>
+      <c r="E57">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58">
+        <v>12</v>
+      </c>
+      <c r="C58">
+        <v>13</v>
+      </c>
+      <c r="D58">
+        <v>12</v>
+      </c>
+      <c r="E58">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>13</v>
+      </c>
+      <c r="D59">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60">
+        <v>12</v>
+      </c>
+      <c r="C60">
+        <v>13</v>
+      </c>
+      <c r="D60">
+        <v>12</v>
+      </c>
+      <c r="E60">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>13</v>
+      </c>
+      <c r="E61">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>13</v>
+      </c>
+      <c r="D62">
+        <v>12</v>
+      </c>
+      <c r="E62">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63">
+        <v>12</v>
+      </c>
+      <c r="C63">
+        <v>13</v>
+      </c>
+      <c r="D63">
+        <v>12</v>
+      </c>
+      <c r="E63">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64">
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="E64">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>68</v>
+      </c>
+      <c r="B65">
+        <v>12</v>
+      </c>
+      <c r="C65">
+        <v>13</v>
+      </c>
+      <c r="D65">
+        <v>12</v>
+      </c>
+      <c r="E65">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66">
+        <v>13</v>
+      </c>
+      <c r="D66">
+        <v>12</v>
+      </c>
+      <c r="E66">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
+      <c r="B67">
+        <v>12</v>
+      </c>
+      <c r="C67">
+        <v>13</v>
+      </c>
+      <c r="D67">
+        <v>12</v>
+      </c>
+      <c r="E67">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68">
+        <v>12</v>
+      </c>
+      <c r="C68">
+        <v>13</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="E68">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69">
+        <v>12</v>
+      </c>
+      <c r="C69">
+        <v>13</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="E69">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70">
+        <v>13</v>
+      </c>
+      <c r="D70">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71">
+        <v>12</v>
+      </c>
+      <c r="C71">
+        <v>13</v>
+      </c>
+      <c r="D71">
+        <v>12</v>
+      </c>
+      <c r="E71">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72">
+        <v>12</v>
+      </c>
+      <c r="C72">
+        <v>13</v>
+      </c>
+      <c r="E72">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+      <c r="B73">
+        <v>12</v>
+      </c>
+      <c r="C73">
+        <v>13</v>
+      </c>
+      <c r="D73">
+        <v>12</v>
+      </c>
+      <c r="E73">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74">
+        <v>12</v>
+      </c>
+      <c r="C74">
+        <v>13</v>
+      </c>
+      <c r="D74">
+        <v>12</v>
+      </c>
+      <c r="E74">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75">
+        <v>12</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="E75">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76">
+        <v>12</v>
+      </c>
+      <c r="C76">
+        <v>13</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>80</v>
+      </c>
+      <c r="C77">
+        <v>13</v>
+      </c>
+      <c r="D77">
+        <v>12</v>
+      </c>
+      <c r="E77">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78">
+        <v>12</v>
+      </c>
+      <c r="C78">
+        <v>13</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="E78">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>82</v>
+      </c>
+      <c r="B79">
+        <v>12</v>
+      </c>
+      <c r="C79">
+        <v>13</v>
+      </c>
+      <c r="D79">
+        <v>12</v>
+      </c>
+      <c r="E79">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80">
+        <v>12</v>
+      </c>
+      <c r="C80">
+        <v>13</v>
+      </c>
+      <c r="D80">
+        <v>12</v>
+      </c>
+      <c r="E80">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="C81">
+        <v>13</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82">
+        <v>12</v>
+      </c>
+      <c r="C82">
+        <v>13</v>
+      </c>
+      <c r="D82">
+        <v>12</v>
+      </c>
+      <c r="E82">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>86</v>
+      </c>
+      <c r="B83">
+        <v>12</v>
+      </c>
+      <c r="C83">
+        <v>13</v>
+      </c>
+      <c r="E83">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>87</v>
+      </c>
+      <c r="B84">
+        <v>12</v>
+      </c>
+      <c r="C84">
+        <v>13</v>
+      </c>
+      <c r="D84">
+        <v>12</v>
+      </c>
+      <c r="E84">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>88</v>
+      </c>
+      <c r="B85">
+        <v>12</v>
+      </c>
+      <c r="C85">
+        <v>13</v>
+      </c>
+      <c r="D85">
+        <v>12</v>
+      </c>
+      <c r="E85">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86">
+        <v>12</v>
+      </c>
+      <c r="D86">
+        <v>12</v>
+      </c>
+      <c r="E86">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87">
+        <v>12</v>
+      </c>
+      <c r="C87">
+        <v>13</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88">
+        <v>13</v>
+      </c>
+      <c r="D88">
+        <v>12</v>
+      </c>
+      <c r="E88">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>92</v>
+      </c>
+      <c r="B89">
+        <v>12</v>
+      </c>
+      <c r="C89">
+        <v>13</v>
+      </c>
+      <c r="D89">
+        <v>12</v>
+      </c>
+      <c r="E89">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>93</v>
+      </c>
+      <c r="B90">
+        <v>12</v>
+      </c>
+      <c r="C90">
+        <v>13</v>
+      </c>
+      <c r="D90">
+        <v>12</v>
+      </c>
+      <c r="E90">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91">
+        <v>12</v>
+      </c>
+      <c r="C91">
+        <v>13</v>
+      </c>
+      <c r="D91">
+        <v>12</v>
+      </c>
+      <c r="E91">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>95</v>
+      </c>
+      <c r="C92">
+        <v>13</v>
+      </c>
+      <c r="D92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93">
+        <v>12</v>
+      </c>
+      <c r="C93">
+        <v>13</v>
+      </c>
+      <c r="D93">
+        <v>12</v>
+      </c>
+      <c r="E93">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>97</v>
+      </c>
+      <c r="B94">
+        <v>12</v>
+      </c>
+      <c r="C94">
+        <v>13</v>
+      </c>
+      <c r="E94">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B95">
+        <v>12</v>
+      </c>
+      <c r="C95">
+        <v>13</v>
+      </c>
+      <c r="D95">
+        <v>12</v>
+      </c>
+      <c r="E95">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+      <c r="B96">
+        <v>12</v>
+      </c>
+      <c r="C96">
+        <v>13</v>
+      </c>
+      <c r="D96">
+        <v>12</v>
+      </c>
+      <c r="E96">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97">
+        <v>12</v>
+      </c>
+      <c r="D97">
+        <v>12</v>
+      </c>
+      <c r="E97">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98">
+        <v>12</v>
+      </c>
+      <c r="C98">
+        <v>13</v>
+      </c>
+      <c r="D98">
+        <v>12</v>
+      </c>
+      <c r="E98">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+      <c r="C99">
+        <v>13</v>
+      </c>
+      <c r="D99">
+        <v>12</v>
+      </c>
+      <c r="E99">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100">
+        <v>12</v>
+      </c>
+      <c r="C100">
+        <v>13</v>
+      </c>
+      <c r="D100">
+        <v>12</v>
+      </c>
+      <c r="E100">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101">
+        <v>12</v>
+      </c>
+      <c r="C101">
+        <v>13</v>
+      </c>
+      <c r="D101">
+        <v>12</v>
+      </c>
+      <c r="E101">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102">
+        <v>12</v>
+      </c>
+      <c r="C102">
+        <v>13</v>
+      </c>
+      <c r="D102">
+        <v>12</v>
+      </c>
+      <c r="E102">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103">
+        <v>13</v>
+      </c>
+      <c r="D103">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>107</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>13</v>
+      </c>
+      <c r="D104">
+        <v>12</v>
+      </c>
+      <c r="E104">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>108</v>
+      </c>
+      <c r="B105">
+        <v>12</v>
+      </c>
+      <c r="C105">
+        <v>13</v>
+      </c>
+      <c r="E105">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>109</v>
+      </c>
+      <c r="B106">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>13</v>
+      </c>
+      <c r="D106">
+        <v>12</v>
+      </c>
+      <c r="E106">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107">
+        <v>12</v>
+      </c>
+      <c r="C107">
+        <v>13</v>
+      </c>
+      <c r="D107">
+        <v>12</v>
+      </c>
+      <c r="E107">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>111</v>
+      </c>
+      <c r="B108">
+        <v>12</v>
+      </c>
+      <c r="D108">
+        <v>12</v>
+      </c>
+      <c r="E108">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>112</v>
+      </c>
+      <c r="B109">
+        <v>12</v>
+      </c>
+      <c r="C109">
+        <v>13</v>
+      </c>
+      <c r="D109">
+        <v>12</v>
+      </c>
+      <c r="E109">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>113</v>
+      </c>
+      <c r="C110">
+        <v>13</v>
+      </c>
+      <c r="D110">
+        <v>12</v>
+      </c>
+      <c r="E110">
         <v>13</v>
       </c>
     </row>

</xml_diff>